<commit_message>
correct ev charging switch issue
</commit_message>
<xml_diff>
--- a/database/data.xlsx
+++ b/database/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Code\ev-fleet-management\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Code\ev_fleet_charging\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA1329F-347F-4D67-BEB7-F74A5EA772F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E4D3E5-4D01-46D4-B73D-B359F17002CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicles" sheetId="14" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>List of required parameters</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>EVCS3_3</t>
-  </si>
-  <si>
-    <t>Ac</t>
   </si>
   <si>
     <t>Unauthorized</t>
@@ -2212,7 +2209,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2413,7 +2410,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2445,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC184BF-3A0B-4706-9CB5-90B38A92B757}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2510,7 +2507,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C6" s="31">
         <v>7</v>
@@ -2606,7 +2603,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7668,8 +7665,8 @@
   </sheetPr>
   <dimension ref="A1:F985"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7794,7 +7791,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="22">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10757,8 +10754,8 @@
   </sheetPr>
   <dimension ref="A1:B976"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>